<commit_message>
Minor edits to sheets.
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/glioblastoma_100cells.xlsx
+++ b/infrastructure_testing_files/current/glioblastoma_100cells.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{343E39EE-FAA9-6E48-9B88-8ABCAD22B18D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3F99CA2C-6E30-1046-8DCC-35DBAA257A7D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25300" yWindow="460" windowWidth="25720" windowHeight="16700" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25300" yWindow="460" windowWidth="25720" windowHeight="16700" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,14 @@
     <sheet name="Dissociation protocol" sheetId="11" r:id="rId7"/>
     <sheet name="Library preparation protocol" sheetId="13" r:id="rId8"/>
     <sheet name="Sequencing protocol" sheetId="14" r:id="rId9"/>
+    <sheet name="Schemas" sheetId="15" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3009" uniqueCount="1251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3032" uniqueCount="1273">
   <si>
     <t>A unique label for the project.</t>
   </si>
@@ -3781,6 +3782,72 @@
   </si>
   <si>
     <t>EFO:0008441</t>
+  </si>
+  <si>
+    <t>Schemas</t>
+  </si>
+  <si>
+    <t>http://schema.dev.data.humancellatlas.org/type/protocol/6.3.3/protocol</t>
+  </si>
+  <si>
+    <t>http://schema.dev.data.humancellatlas.org/type/protocol/biomaterial_collection/8.2.4/collection_protocol</t>
+  </si>
+  <si>
+    <t>http://schema.dev.data.humancellatlas.org/type/protocol/biomaterial_collection/1.2.4/differentiation_protocol</t>
+  </si>
+  <si>
+    <t>http://schema.dev.data.humancellatlas.org/type/protocol/biomaterial_collection/1.2.4/ipsc_induction_protocol</t>
+  </si>
+  <si>
+    <t>http://schema.dev.data.humancellatlas.org/type/protocol/biomaterial_collection/1.1.3/aggregate_generation_protocol</t>
+  </si>
+  <si>
+    <t>http://schema.dev.data.humancellatlas.org/type/protocol/biomaterial_collection/4.2.4/dissociation_protocol</t>
+  </si>
+  <si>
+    <t>http://schema.dev.data.humancellatlas.org/type/protocol/biomaterial_collection/2.2.3/enrichment_protocol</t>
+  </si>
+  <si>
+    <t>http://schema.dev.data.humancellatlas.org/type/protocol/sequencing/4.2.5/library_preparation_protocol</t>
+  </si>
+  <si>
+    <t>http://schema.dev.data.humancellatlas.org/type/protocol/sequencing/8.1.1/sequencing_protocol</t>
+  </si>
+  <si>
+    <t>http://schema.dev.data.humancellatlas.org/type/protocol/analysis/7.2.4/analysis_protocol</t>
+  </si>
+  <si>
+    <t>http://schema.dev.data.humancellatlas.org/type/protocol/imaging/7.2.2/imaging_protocol</t>
+  </si>
+  <si>
+    <t>http://schema.dev.data.humancellatlas.org/type/biomaterial/8.3.6/cell_suspension</t>
+  </si>
+  <si>
+    <t>http://schema.dev.data.humancellatlas.org/type/biomaterial/6.2.6/specimen_from_organism</t>
+  </si>
+  <si>
+    <t>http://schema.dev.data.humancellatlas.org/type/biomaterial/8.3.6/cell_line</t>
+  </si>
+  <si>
+    <t>http://schema.dev.data.humancellatlas.org/type/biomaterial/8.2.7/donor_organism</t>
+  </si>
+  <si>
+    <t>http://schema.dev.data.humancellatlas.org/type/biomaterial/8.3.3/organoid</t>
+  </si>
+  <si>
+    <t>http://schema.dev.data.humancellatlas.org/type/file/5.3.2/analysis_file</t>
+  </si>
+  <si>
+    <t>http://schema.dev.data.humancellatlas.org/type/file/2.2.3/reference_file</t>
+  </si>
+  <si>
+    <t>http://schema.dev.data.humancellatlas.org/type/file/6.3.3/sequence_file</t>
+  </si>
+  <si>
+    <t>http://schema.dev.data.humancellatlas.org/type/project/8.2.6/project</t>
+  </si>
+  <si>
+    <t>http://schema.dev.data.humancellatlas.org/type/process/4.2.4/process</t>
   </si>
 </sst>
 </file>
@@ -3889,14 +3956,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3918,9 +3989,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink 2" xfId="2" xr:uid="{15B98A4B-5127-0B4E-A677-E2EA4BA17812}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4399,6 +4472,160 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E526EF6D-29D8-7D4A-A6AC-B6356AF2D52D}">
+  <dimension ref="A1:A23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="15" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="15" t="s">
+        <v>1262</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="15" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="15" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="15" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="15" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="15" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="15" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="15" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="15" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{3A3E4655-C484-8244-AD4F-9042D91462BA}"/>
+    <hyperlink ref="A11" r:id="rId2" xr:uid="{DF359B20-7FD9-5E48-B06C-295B0F26820F}"/>
+    <hyperlink ref="A14" r:id="rId3" xr:uid="{B1461DAC-3F96-EC44-94DC-0A6BAA07E332}"/>
+    <hyperlink ref="A21" r:id="rId4" xr:uid="{BBC892BE-9F8E-A046-9A04-E1FD2401137A}"/>
+    <hyperlink ref="A2" r:id="rId5" xr:uid="{8BDFB560-3025-1F42-8360-2B3FEE2F0966}"/>
+    <hyperlink ref="A12" r:id="rId6" xr:uid="{2682FA0C-DBA9-ED4D-BF50-B9F9C4B787BB}"/>
+    <hyperlink ref="A13" r:id="rId7" xr:uid="{EBC1903D-3FDC-ED4B-B236-A22E87F8EFBF}"/>
+    <hyperlink ref="A15" r:id="rId8" xr:uid="{9BB615A5-969F-014B-A171-94ACC6CB7A91}"/>
+    <hyperlink ref="A16" r:id="rId9" xr:uid="{293339C0-995B-E444-B80D-C58457C654F2}"/>
+    <hyperlink ref="A17" r:id="rId10" xr:uid="{165E67E7-1C3F-4249-9F10-644A3DBA5FCA}"/>
+    <hyperlink ref="A18" r:id="rId11" xr:uid="{F60CA28C-94B9-6646-B385-E85AF8610975}"/>
+    <hyperlink ref="A19" r:id="rId12" xr:uid="{56ADF6E0-3DA7-844F-BE19-5877D56B0C6C}"/>
+    <hyperlink ref="A22" r:id="rId13" xr:uid="{64B782C6-50F9-7E4A-A104-6B46AA9AD4D3}"/>
+    <hyperlink ref="A9" r:id="rId14" xr:uid="{D8C63F49-82D3-B448-BAE7-87CD9C40AC0C}"/>
+    <hyperlink ref="A10" r:id="rId15" xr:uid="{0E7E6990-5FBA-F34E-BC55-5DD5F1A151DA}"/>
+    <hyperlink ref="A23" r:id="rId16" xr:uid="{1A67BF9D-64B3-294F-A4E9-CE01A99532F7}"/>
+    <hyperlink ref="A7" r:id="rId17" xr:uid="{49650D85-348D-ED49-9D5F-890DEBCE3E57}"/>
+    <hyperlink ref="A8" r:id="rId18" xr:uid="{C74231F2-0050-2D44-B796-019ED39E08F6}"/>
+    <hyperlink ref="A20" r:id="rId19" xr:uid="{DC1681E1-95EB-6344-96EB-DF5D010A73DF}"/>
+    <hyperlink ref="A4" r:id="rId20" xr:uid="{B38B5F37-53C8-CA40-B7E0-506071A2B45A}"/>
+    <hyperlink ref="A5" r:id="rId21" xr:uid="{B1EFD83A-A420-F247-A3E6-8DA14B817E13}"/>
+    <hyperlink ref="A6" r:id="rId22" xr:uid="{128F9969-1A72-1B4F-B1F2-2CF9564BB253}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I6"/>
@@ -20588,7 +20815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K6" sqref="K6:L6"/>
     </sheetView>
   </sheetViews>

</xml_diff>